<commit_message>
con chorme driver acutalizdo
</commit_message>
<xml_diff>
--- a/src/test/resources/dataDriven/LRETAMOZO/DataPrueba.xlsx
+++ b/src/test/resources/dataDriven/LRETAMOZO/DataPrueba.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse_WS\Geolocalizacion\P-Geo\src\test\resources\dataDriven\LRETAMOZO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse_WS\GeoSinDependencia\Geolocalizacion_SinDependencia\src\test\resources\dataDriven\LRETAMOZO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9852AC-15D1-4946-AE79-9CF3454AC22A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA967123-D40E-41E5-ACE3-FA43DF5C02F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01-RegistrarAtencion" sheetId="1" r:id="rId1"/>
     <sheet name="02-AsignarProcurador" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="43">
   <si>
     <t>usar</t>
   </si>
@@ -61,27 +61,9 @@
     <t>Test2019#</t>
   </si>
   <si>
-    <t>ROCIO PAREDES</t>
-  </si>
-  <si>
-    <t>PRUEBAS2 LEGALL LEGALL</t>
-  </si>
-  <si>
     <t>En camino</t>
   </si>
   <si>
-    <t>ABA070</t>
-  </si>
-  <si>
-    <t>ABA071</t>
-  </si>
-  <si>
-    <t>ABA072</t>
-  </si>
-  <si>
-    <t>ABA073</t>
-  </si>
-  <si>
     <t>telefono</t>
   </si>
   <si>
@@ -137,6 +119,48 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ABA300</t>
+  </si>
+  <si>
+    <t>ABA301</t>
+  </si>
+  <si>
+    <t>ABA302</t>
+  </si>
+  <si>
+    <t>ABA303</t>
+  </si>
+  <si>
+    <t>ABA304</t>
+  </si>
+  <si>
+    <t>ABA305</t>
+  </si>
+  <si>
+    <t>ABA306</t>
+  </si>
+  <si>
+    <t>ABA307</t>
+  </si>
+  <si>
+    <t>ABA308</t>
+  </si>
+  <si>
+    <t>PROCURADOR AUTO5</t>
+  </si>
+  <si>
+    <t>PROCURADOR AUTO1</t>
+  </si>
+  <si>
+    <t>PROCURADOR AUTO2</t>
+  </si>
+  <si>
+    <t>PROCURADOR AUTO3</t>
+  </si>
+  <si>
+    <t>PROCURADOR AUTO4</t>
   </si>
 </sst>
 </file>
@@ -593,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +631,8 @@
     <col min="6" max="6" width="33.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="1017" width="9.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="1017" width="9.109375" style="1" customWidth="1"/>
     <col min="1018" max="1024" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -625,301 +650,310 @@
         <v>4</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="J5" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="J6" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="G9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="I10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -938,16 +972,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBAA0A67-BA6C-453E-9BA4-3083C2316444}">
-  <dimension ref="A1:AMD5"/>
+  <dimension ref="A1:AMD6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:A5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="1018" width="9.109375" style="1" customWidth="1"/>
     <col min="1019" max="1025" width="9.109375" customWidth="1"/>
@@ -985,13 +1021,13 @@
       </c>
       <c r="D2" s="1" t="str">
         <f>'01-RegistrarAtencion'!D2</f>
-        <v>ABA070</v>
+        <v>ABA300</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1006,13 +1042,13 @@
       </c>
       <c r="D3" s="1" t="str">
         <f>'01-RegistrarAtencion'!D3</f>
-        <v>ABA071</v>
+        <v>ABA301</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1027,13 +1063,13 @@
       </c>
       <c r="D4" s="1" t="str">
         <f>'01-RegistrarAtencion'!D4</f>
-        <v>ABA072</v>
+        <v>ABA302</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1048,21 +1084,44 @@
       </c>
       <c r="D5" s="1" t="str">
         <f>'01-RegistrarAtencion'!D5</f>
-        <v>ABA073</v>
+        <v>ABA303</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>'01-RegistrarAtencion'!D6</f>
+        <v>ABA304</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F38DA22A-F66F-48EF-A246-7CC780DC453E}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{539B428D-6F6D-4E7B-9E08-F978316EE028}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{555577FD-DEB6-4943-9200-0A97263081AC}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{3BEB8098-14A3-41BE-ADE5-52226F072453}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{713344E3-E12B-4158-8BE7-333ACFBB4B13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>